<commit_message>
4th draft update py3.8_ opencv not fin
</commit_message>
<xml_diff>
--- a/require file/key_2020FEST.xlsx
+++ b/require file/key_2020FEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Window\Desktop\FE camp\fe coding\Exam Checker_img pro_final\require file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D7516-B55C-4184-88F6-AB59E69E3DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347710B1-A537-434E-81C2-A80CCD949597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{77391108-DAB4-440E-8224-F97C51C486BF}"/>
   </bookViews>
@@ -28,6 +28,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+  <si>
+    <t>free</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8172A5-FD6E-4868-B160-9E99B4BCBD0E}">
   <dimension ref="A1:BR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BO11" sqref="BO11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -627,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2">
         <v>2</v>
@@ -668,8 +676,8 @@
       <c r="W2">
         <v>2</v>
       </c>
-      <c r="X2">
-        <v>1</v>
+      <c r="X2" t="s">
+        <v>0</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -749,8 +757,8 @@
       <c r="AX2">
         <v>1</v>
       </c>
-      <c r="AY2">
-        <v>5</v>
+      <c r="AY2" t="s">
+        <v>0</v>
       </c>
       <c r="AZ2">
         <v>3</v>
@@ -779,8 +787,8 @@
       <c r="BH2">
         <v>1</v>
       </c>
-      <c r="BI2">
-        <v>4</v>
+      <c r="BI2" t="s">
+        <v>0</v>
       </c>
       <c r="BJ2">
         <v>111.11</v>
@@ -798,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="BO2">
-        <v>3</v>
+        <v>0.33</v>
       </c>
       <c r="BP2">
         <v>4</v>

</xml_diff>